<commit_message>
Add 24/07/16 47 lines
</commit_message>
<xml_diff>
--- a/deck_improvement_DataBase.xlsx
+++ b/deck_improvement_DataBase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danil\Documents\Projetos_Portifolio\Otimizando_Deck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415B0063-0415-4FDE-A92D-394186B8DA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F278469-7C64-4D38-AEA6-0A3393505E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{42FCC64A-8D20-4B04-8DAD-AC986B83D54C}"/>
   </bookViews>
@@ -16,17 +16,226 @@
     <sheet name="otim_deck" sheetId="1" r:id="rId1"/>
     <sheet name="deck_v1.0" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="101">
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>against</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>how</t>
+  </si>
+  <si>
+    <t>specified</t>
+  </si>
+  <si>
+    <t>obs</t>
+  </si>
+  <si>
+    <t>my life total</t>
+  </si>
+  <si>
+    <t>opponent life total</t>
+  </si>
+  <si>
+    <t>v1.0</t>
+  </si>
+  <si>
+    <t>izzet artefatos</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>win</t>
+  </si>
+  <si>
+    <t>concede</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>izzet phoenix</t>
+  </si>
+  <si>
+    <t>opponent</t>
+  </si>
+  <si>
+    <t>lose</t>
+  </si>
+  <si>
+    <t>life total</t>
+  </si>
+  <si>
+    <t>combat damage</t>
+  </si>
+  <si>
+    <t>slow</t>
+  </si>
+  <si>
+    <t>mono red kuldotha</t>
+  </si>
+  <si>
+    <t>direct damage</t>
+  </si>
+  <si>
+    <t>life loss</t>
+  </si>
+  <si>
+    <t>5c</t>
+  </si>
+  <si>
+    <t>flood</t>
+  </si>
+  <si>
+    <t>rakdos sacrifice</t>
+  </si>
+  <si>
+    <t>life drain</t>
+  </si>
+  <si>
+    <t>zika</t>
+  </si>
+  <si>
+    <t>dimir control mill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">me </t>
+  </si>
+  <si>
+    <t>deck over</t>
+  </si>
+  <si>
+    <t>mill</t>
+  </si>
+  <si>
+    <t>mono red magos</t>
+  </si>
+  <si>
+    <t>4c</t>
+  </si>
+  <si>
+    <t>discard</t>
+  </si>
+  <si>
+    <t>rakdos vampires</t>
+  </si>
+  <si>
+    <t>board wipe</t>
+  </si>
+  <si>
+    <t>mono green devotion</t>
+  </si>
+  <si>
+    <t>selesnya enchantments</t>
+  </si>
+  <si>
+    <t>sultai ultimatum</t>
+  </si>
+  <si>
+    <t>izzet counters</t>
+  </si>
+  <si>
+    <t>rakdos joins up combo</t>
+  </si>
+  <si>
+    <t>boros convoke</t>
+  </si>
+  <si>
+    <t>gruul legends</t>
+  </si>
+  <si>
+    <t>mono black discard</t>
+  </si>
+  <si>
+    <t>5c domain</t>
+  </si>
+  <si>
+    <t>mono white life gain</t>
+  </si>
+  <si>
+    <t>gruul stompy</t>
+  </si>
+  <si>
+    <t>rakdos midrange</t>
+  </si>
+  <si>
+    <t>fractius</t>
+  </si>
+  <si>
+    <t>poison</t>
+  </si>
+  <si>
+    <t>goblins</t>
+  </si>
+  <si>
+    <t>rakdos aggro</t>
+  </si>
+  <si>
+    <t>mono white anjos</t>
+  </si>
+  <si>
+    <t>dredge</t>
+  </si>
+  <si>
+    <t>selesnya counters</t>
+  </si>
+  <si>
+    <t>simic flash</t>
+  </si>
+  <si>
+    <t>mono green stompy</t>
+  </si>
+  <si>
+    <t>elves</t>
+  </si>
+  <si>
+    <t>mardu knight</t>
+  </si>
+  <si>
+    <t>mono blue mill</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>orzhov discard</t>
+  </si>
+  <si>
+    <t>abzan greasefang</t>
+  </si>
   <si>
     <t>qtd</t>
   </si>
@@ -91,12 +300,12 @@
     <t>Fatal Push</t>
   </si>
   <si>
+    <t>instant</t>
+  </si>
+  <si>
     <t>Claim the Firstborn</t>
   </si>
   <si>
-    <t>instant</t>
-  </si>
-  <si>
     <t>Deadly Dispute</t>
   </si>
   <si>
@@ -131,205 +340,13 @@
   </si>
   <si>
     <t>companion</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>how</t>
-  </si>
-  <si>
-    <t>against</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>specified</t>
-  </si>
-  <si>
-    <t>hand</t>
-  </si>
-  <si>
-    <t>izzet artefatos</t>
-  </si>
-  <si>
-    <t>v1.0</t>
-  </si>
-  <si>
-    <t>win</t>
-  </si>
-  <si>
-    <t>concede</t>
-  </si>
-  <si>
-    <t>my life total</t>
-  </si>
-  <si>
-    <t>opponent life total</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>izzet phoenix</t>
-  </si>
-  <si>
-    <t>life total</t>
-  </si>
-  <si>
-    <t>combat damage</t>
-  </si>
-  <si>
-    <t>lose</t>
-  </si>
-  <si>
-    <t>me</t>
-  </si>
-  <si>
-    <t>opponent</t>
-  </si>
-  <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>mono red kuldotha</t>
-  </si>
-  <si>
-    <t>direct damage</t>
-  </si>
-  <si>
-    <t>obs</t>
-  </si>
-  <si>
-    <t>flood</t>
-  </si>
-  <si>
-    <t>life loss</t>
-  </si>
-  <si>
-    <t>slow</t>
-  </si>
-  <si>
-    <t>5c</t>
-  </si>
-  <si>
-    <t>zika</t>
-  </si>
-  <si>
-    <t>life drain</t>
-  </si>
-  <si>
-    <t>rakdos sacrifice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">me </t>
-  </si>
-  <si>
-    <t>dimir control mill</t>
-  </si>
-  <si>
-    <t>deck over</t>
-  </si>
-  <si>
-    <t>mill</t>
-  </si>
-  <si>
-    <t>mono red magos</t>
-  </si>
-  <si>
-    <t>discard</t>
-  </si>
-  <si>
-    <t>4c</t>
-  </si>
-  <si>
-    <t>rakdos vampires</t>
-  </si>
-  <si>
-    <t>board wipe</t>
-  </si>
-  <si>
-    <t>mono green devotion</t>
-  </si>
-  <si>
-    <t>selesnya enchantments</t>
-  </si>
-  <si>
-    <t>sultai ultimatum</t>
-  </si>
-  <si>
-    <t>izzet counters</t>
-  </si>
-  <si>
-    <t>rakdos joins up combo</t>
-  </si>
-  <si>
-    <t>boros convoke</t>
-  </si>
-  <si>
-    <t>gruul legends</t>
-  </si>
-  <si>
-    <t>mono black discard</t>
-  </si>
-  <si>
-    <t>5c domain</t>
-  </si>
-  <si>
-    <t>mono white life gain</t>
-  </si>
-  <si>
-    <t>gruul stompy</t>
-  </si>
-  <si>
-    <t>rakdos midrange</t>
-  </si>
-  <si>
-    <t>fractius</t>
-  </si>
-  <si>
-    <t>poison</t>
-  </si>
-  <si>
-    <t>goblins</t>
-  </si>
-  <si>
-    <t>rakdos aggro</t>
-  </si>
-  <si>
-    <t>mono white anjos</t>
-  </si>
-  <si>
-    <t>dredge</t>
-  </si>
-  <si>
-    <t>selesnya counters</t>
-  </si>
-  <si>
-    <t>simic flash</t>
-  </si>
-  <si>
-    <t>mono green stompy</t>
-  </si>
-  <si>
-    <t>elves</t>
-  </si>
-  <si>
-    <t>mardu knight</t>
-  </si>
-  <si>
-    <t>mono blue mill</t>
-  </si>
-  <si>
-    <t>red</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,7 +407,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -686,11 +703,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496ACE0D-7759-403F-9FD1-141A18E1771B}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -700,62 +717,62 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I2" s="1">
         <v>19</v>
@@ -764,30 +781,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1">
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -796,30 +813,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1">
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
@@ -828,30 +845,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="I5" s="1">
         <v>6</v>
@@ -860,30 +877,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1">
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
@@ -892,30 +909,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1">
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I7" s="1">
         <v>19</v>
@@ -924,30 +941,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1">
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -956,30 +973,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1">
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="I9" s="1">
         <v>15</v>
@@ -988,30 +1005,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1">
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I10" s="1">
         <v>11</v>
@@ -1020,30 +1037,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1">
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
@@ -1052,30 +1069,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1">
         <v>6</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="I12" s="1">
         <v>15</v>
@@ -1084,30 +1101,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1">
         <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I13" s="1">
         <v>18</v>
@@ -1116,30 +1133,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1">
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
@@ -1148,30 +1165,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1">
         <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I15" s="1">
         <v>5</v>
@@ -1180,30 +1197,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1">
         <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="I16" s="1">
         <v>6</v>
@@ -1212,30 +1229,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1">
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I17" s="1">
         <v>11</v>
@@ -1244,30 +1261,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D18" s="1">
         <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I18" s="1">
         <v>7</v>
@@ -1276,94 +1293,94 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D19" s="1">
         <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="1">
+        <v>13</v>
+      </c>
+      <c r="J19" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I19" s="1">
-        <v>13</v>
-      </c>
-      <c r="J19" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="1">
-        <v>7</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I20" s="1">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1">
         <v>6</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -1372,30 +1389,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1">
         <v>6</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I22" s="1">
         <v>17</v>
@@ -1404,30 +1421,30 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D23" s="1">
         <v>6</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="I23" s="1">
         <v>6</v>
@@ -1436,30 +1453,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D24" s="1">
         <v>7</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I24" s="1">
         <v>22</v>
@@ -1468,30 +1485,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D25" s="1">
         <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I25" s="1">
         <v>17</v>
@@ -1500,30 +1517,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D26" s="1">
         <v>7</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I26" s="1">
         <v>14</v>
@@ -1532,30 +1549,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="1">
+        <v>7</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="1">
-        <v>7</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I27" s="1">
         <v>10</v>
@@ -1564,30 +1581,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D28" s="1">
         <v>6</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="I28" s="1">
         <v>20</v>
@@ -1596,30 +1613,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D29" s="1">
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I29" s="1">
         <v>2</v>
@@ -1628,30 +1645,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D30" s="1">
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I30" s="1">
         <v>0</v>
@@ -1660,30 +1677,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D31" s="1">
         <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I31" s="1">
         <v>17</v>
@@ -1692,30 +1709,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D32" s="1">
         <v>7</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I32" s="1">
         <v>21</v>
@@ -1724,30 +1741,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D33" s="1">
         <v>6</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="I33" s="1">
         <v>0</v>
@@ -1756,30 +1773,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D34" s="1">
         <v>7</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I34" s="1">
         <v>0</v>
@@ -1788,30 +1805,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D35" s="1">
         <v>6</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
@@ -1820,30 +1837,30 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D36" s="1">
         <v>6</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I36" s="1">
         <v>21</v>
@@ -1852,30 +1869,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1">
         <v>7</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I37" s="1">
         <v>15</v>
@@ -1884,30 +1901,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D38" s="1">
         <v>7</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I38" s="1">
         <v>20</v>
@@ -1916,30 +1933,30 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D39" s="1">
         <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I39" s="1">
         <v>21</v>
@@ -1948,30 +1965,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D40" s="1">
         <v>7</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="I40" s="1">
         <v>11</v>
@@ -1980,30 +1997,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D41" s="1">
         <v>7</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="I41" s="1">
         <v>21</v>
@@ -2012,30 +2029,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D42" s="1">
         <v>7</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I42" s="1">
         <v>15</v>
@@ -2044,36 +2061,196 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D43" s="1">
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I43" s="1">
         <v>20</v>
       </c>
       <c r="J43" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="1">
+        <v>7</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" s="1">
+        <v>19</v>
+      </c>
+      <c r="J44" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="1">
+        <v>7</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="1">
+        <v>7</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I46" s="1">
+        <v>18</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="1">
+        <v>7</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="1">
+        <v>20</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" s="1">
+        <v>6</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0</v>
+      </c>
+      <c r="J48" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2089,7 +2266,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="28.140625" style="1" bestFit="1" customWidth="1"/>
@@ -2098,340 +2275,340 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>